<commit_message>
updated deaths and dalys
</commit_message>
<xml_diff>
--- a/Lit review data/deaths and dalys.xlsx
+++ b/Lit review data/deaths and dalys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/Lit review data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FB5B76F-82F9-7841-8962-2108D1D7978F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC230842-06E0-8942-B71F-0A961BE02A5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="27640" windowHeight="16100" activeTab="1" xr2:uid="{2FD00656-5231-DE49-A742-F6C9FCCF5F37}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27640" windowHeight="16100" activeTab="1" xr2:uid="{2FD00656-5231-DE49-A742-F6C9FCCF5F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="189">
   <si>
     <t>species</t>
   </si>
@@ -615,12 +615,6 @@
   </si>
   <si>
     <t xml:space="preserve">number of studies </t>
-  </si>
-  <si>
-    <t>8 (though this does not include studies that don't specify hookworm)</t>
-  </si>
-  <si>
-    <t>90 (though this does not include studies that don't specify LF)</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{095D0EB1-2098-4240-8E83-2B860324C729}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -1660,7 +1654,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1739,8 +1733,8 @@
       <c r="B3" t="s">
         <v>87</v>
       </c>
-      <c r="C3" t="s">
-        <v>190</v>
+      <c r="C3">
+        <v>100</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -2087,8 +2081,8 @@
       <c r="B15" t="s">
         <v>88</v>
       </c>
-      <c r="C15" t="s">
-        <v>189</v>
+      <c r="C15">
+        <v>68</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>

</xml_diff>